<commit_message>
Fix bug with duplicate rows
</commit_message>
<xml_diff>
--- a/InterfaceLab2/result.xlsx
+++ b/InterfaceLab2/result.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dev\hci\InterfaceLab1\InterfaceLab2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{E67791C7-39EA-4A8F-A4A3-7321DFAB843C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{311552C0-0444-43DC-9462-4105363E0916}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3552" yWindow="36" windowWidth="19488" windowHeight="11784"/>
   </bookViews>
@@ -651,9 +651,45 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-            <c:trendlineType val="linear"/>
+            <c:trendlineType val="log"/>
             <c:dispRSqr val="0"/>
-            <c:dispEq val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-3.5251807989445841E-2"/>
+                  <c:y val="-6.3750971434718653E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="ru-RU"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
           </c:trendline>
           <c:val>
             <c:numRef>
@@ -1743,8 +1779,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" workbookViewId="0">
-      <selection activeCell="F35" sqref="F35"/>
+    <sheetView tabSelected="1" zoomScale="106" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Task 2 part 2 final
</commit_message>
<xml_diff>
--- a/InterfaceLab2/result.xlsx
+++ b/InterfaceLab2/result.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,19 +8,31 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dev\hci\InterfaceLab1\InterfaceLab2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{311552C0-0444-43DC-9462-4105363E0916}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD2155AB-B0F5-4E80-AA97-7D245FE12BE7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3552" yWindow="36" windowWidth="19488" windowHeight="11784"/>
+    <workbookView xWindow="2496" yWindow="144" windowWidth="19488" windowHeight="11784" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
+    <sheet name="Часть 1" sheetId="1" r:id="rId1"/>
+    <sheet name="Часть 2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Среднее время</t>
   </si>
@@ -30,11 +42,50 @@
   <si>
     <t>Попытки</t>
   </si>
+  <si>
+    <t>Font size: 10</t>
+  </si>
+  <si>
+    <t>Font size: 11</t>
+  </si>
+  <si>
+    <t>Font size: 12</t>
+  </si>
+  <si>
+    <t>Font size: 14</t>
+  </si>
+  <si>
+    <t>Font size: 16</t>
+  </si>
+  <si>
+    <t>Число элементов</t>
+  </si>
+  <si>
+    <t>Color: #FFDC143C (желтый)</t>
+  </si>
+  <si>
+    <t>Color: #FF0000FF (красный)</t>
+  </si>
+  <si>
+    <t>Color: #FF008000 (белый)</t>
+  </si>
+  <si>
+    <t>Color: #FFFFFF00 (чёрный)</t>
+  </si>
+  <si>
+    <t>Color: #FF0000FF (синий)</t>
+  </si>
+  <si>
+    <t>Color: #FF008000 (зелёный)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="0.000"/>
+  </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -530,7 +581,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -538,6 +589,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -693,7 +745,7 @@
           </c:trendline>
           <c:val>
             <c:numRef>
-              <c:f>'Sheet 1'!$H$3:$H$8</c:f>
+              <c:f>'Часть 1'!$H$3:$H$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -1776,11 +1828,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="106" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+    <sheetView zoomScale="106" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1977,4 +2029,463 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A1E10AB-FFC3-481A-B985-6CE273AB2EE0}">
+  <dimension ref="B2:I27"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K15" sqref="K15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="29.5546875" customWidth="1"/>
+    <col min="3" max="9" width="9.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="C2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+    </row>
+    <row r="3" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="D3">
+        <v>3</v>
+      </c>
+      <c r="E3">
+        <v>4</v>
+      </c>
+      <c r="F3">
+        <v>5</v>
+      </c>
+      <c r="G3">
+        <v>6</v>
+      </c>
+      <c r="H3">
+        <v>7</v>
+      </c>
+      <c r="I3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="3">
+        <v>1004.9030749999999</v>
+      </c>
+      <c r="D4" s="3">
+        <v>1330.670875</v>
+      </c>
+      <c r="E4" s="3">
+        <v>1238.127675</v>
+      </c>
+      <c r="F4" s="3">
+        <v>1198.59285</v>
+      </c>
+      <c r="G4" s="3">
+        <v>1745.366125</v>
+      </c>
+      <c r="H4" s="3">
+        <v>1229.279025</v>
+      </c>
+      <c r="I4" s="3">
+        <v>1722.786975</v>
+      </c>
+    </row>
+    <row r="5" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="3">
+        <v>1074.6556250000001</v>
+      </c>
+      <c r="D5" s="3">
+        <v>1027.6106749999999</v>
+      </c>
+      <c r="E5" s="3">
+        <v>1332.3396</v>
+      </c>
+      <c r="F5" s="3">
+        <v>1338.6590249999999</v>
+      </c>
+      <c r="G5" s="3">
+        <v>1272.5835999999999</v>
+      </c>
+      <c r="H5" s="3">
+        <v>1479.7436499999999</v>
+      </c>
+      <c r="I5" s="3">
+        <v>1517.6735000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="3">
+        <v>1179.16085</v>
+      </c>
+      <c r="D6" s="3">
+        <v>1171.422425</v>
+      </c>
+      <c r="E6" s="3">
+        <v>1175.671225</v>
+      </c>
+      <c r="F6" s="3">
+        <v>1422.7576750000001</v>
+      </c>
+      <c r="G6" s="3">
+        <v>1569.959175</v>
+      </c>
+      <c r="H6" s="3">
+        <v>1202.4202</v>
+      </c>
+      <c r="I6" s="3">
+        <v>1485.357</v>
+      </c>
+    </row>
+    <row r="7" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="3">
+        <v>1032.783725</v>
+      </c>
+      <c r="D7" s="3">
+        <v>1105.4110000000001</v>
+      </c>
+      <c r="E7" s="3">
+        <v>1388.0989500000001</v>
+      </c>
+      <c r="F7" s="3">
+        <v>1362.5546750000001</v>
+      </c>
+      <c r="G7" s="3">
+        <v>1405.97495</v>
+      </c>
+      <c r="H7" s="3">
+        <v>1758.4484749999999</v>
+      </c>
+      <c r="I7" s="3">
+        <v>2350.2033750000001</v>
+      </c>
+    </row>
+    <row r="8" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="3">
+        <v>951.31907999999999</v>
+      </c>
+      <c r="D8" s="3">
+        <v>1010.75762</v>
+      </c>
+      <c r="E8" s="3">
+        <v>1074.28736</v>
+      </c>
+      <c r="F8" s="3">
+        <v>1276.26386</v>
+      </c>
+      <c r="G8" s="3">
+        <v>1360.31386</v>
+      </c>
+      <c r="H8" s="3">
+        <v>1573.9979000000001</v>
+      </c>
+      <c r="I8" s="3">
+        <v>1730.8684599999999</v>
+      </c>
+    </row>
+    <row r="9" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" s="3">
+        <v>972.47587999999996</v>
+      </c>
+      <c r="D9" s="3">
+        <v>1072.9439400000001</v>
+      </c>
+      <c r="E9" s="3">
+        <v>1178.1591000000001</v>
+      </c>
+      <c r="F9" s="3">
+        <v>1178.40966</v>
+      </c>
+      <c r="G9" s="3">
+        <v>1465.9900399999999</v>
+      </c>
+      <c r="H9" s="3">
+        <v>1472.21336</v>
+      </c>
+      <c r="I9" s="3">
+        <v>1787.4123999999999</v>
+      </c>
+    </row>
+    <row r="10" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B10" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10" s="3">
+        <v>1065.4156499999999</v>
+      </c>
+      <c r="D10" s="3">
+        <v>1016.1310999999999</v>
+      </c>
+      <c r="E10" s="3">
+        <v>1884.7313750000001</v>
+      </c>
+      <c r="F10" s="3">
+        <v>1465.0410750000001</v>
+      </c>
+      <c r="G10" s="3">
+        <v>1691.3992249999999</v>
+      </c>
+      <c r="H10" s="3">
+        <v>1281.9749750000001</v>
+      </c>
+      <c r="I10" s="3">
+        <v>2054.7696999999998</v>
+      </c>
+    </row>
+    <row r="11" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B11" t="s">
+        <v>4</v>
+      </c>
+      <c r="C11" s="3">
+        <v>1513.7846750000001</v>
+      </c>
+      <c r="D11" s="3">
+        <v>1255.6107500000001</v>
+      </c>
+      <c r="E11" s="3">
+        <v>1198.5342499999999</v>
+      </c>
+      <c r="F11" s="3">
+        <v>1638.59935</v>
+      </c>
+      <c r="G11" s="3">
+        <v>1511.56295</v>
+      </c>
+      <c r="H11" s="3">
+        <v>1500.3694499999999</v>
+      </c>
+      <c r="I11" s="3">
+        <v>2063.0205249999999</v>
+      </c>
+    </row>
+    <row r="12" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B12" t="s">
+        <v>5</v>
+      </c>
+      <c r="C12" s="3">
+        <v>1257.4621</v>
+      </c>
+      <c r="D12" s="3">
+        <v>1309.865675</v>
+      </c>
+      <c r="E12" s="3">
+        <v>1184.672225</v>
+      </c>
+      <c r="F12" s="3">
+        <v>1243.9981499999999</v>
+      </c>
+      <c r="G12" s="3">
+        <v>1571.94885</v>
+      </c>
+      <c r="H12" s="3">
+        <v>1954.717725</v>
+      </c>
+      <c r="I12" s="3">
+        <v>1276.023375</v>
+      </c>
+    </row>
+    <row r="13" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B13" t="s">
+        <v>6</v>
+      </c>
+      <c r="C13" s="3">
+        <v>1104.8565249999999</v>
+      </c>
+      <c r="D13" s="3">
+        <v>1060.865675</v>
+      </c>
+      <c r="E13" s="3">
+        <v>1149.8115499999999</v>
+      </c>
+      <c r="F13" s="3">
+        <v>1253.4030749999999</v>
+      </c>
+      <c r="G13" s="3">
+        <v>1238.9387999999999</v>
+      </c>
+      <c r="H13" s="3">
+        <v>1136.793375</v>
+      </c>
+      <c r="I13" s="3">
+        <v>1817.0894249999999</v>
+      </c>
+    </row>
+    <row r="14" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B14" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14" s="3">
+        <v>1532.75855</v>
+      </c>
+      <c r="D14" s="3">
+        <v>955.72614999999996</v>
+      </c>
+      <c r="E14" s="3">
+        <v>1449.186175</v>
+      </c>
+      <c r="F14" s="3">
+        <v>1628.057425</v>
+      </c>
+      <c r="G14" s="3">
+        <v>1988.47135</v>
+      </c>
+      <c r="H14" s="3">
+        <v>1249.4407249999999</v>
+      </c>
+      <c r="I14" s="3">
+        <v>1814.122775</v>
+      </c>
+    </row>
+    <row r="15" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3"/>
+      <c r="H15" s="3"/>
+      <c r="I15" s="3"/>
+    </row>
+    <row r="16" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
+      <c r="H16" s="3"/>
+      <c r="I16" s="3"/>
+    </row>
+    <row r="17" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
+      <c r="G17" s="3"/>
+      <c r="H17" s="3"/>
+      <c r="I17" s="3"/>
+    </row>
+    <row r="18" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="3"/>
+      <c r="H18" s="3"/>
+      <c r="I18" s="3"/>
+    </row>
+    <row r="19" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3"/>
+      <c r="G19" s="3"/>
+      <c r="H19" s="3"/>
+      <c r="I19" s="3"/>
+    </row>
+    <row r="20" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="C20" s="3"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="3"/>
+      <c r="G20" s="3"/>
+      <c r="H20" s="3"/>
+      <c r="I20" s="3"/>
+    </row>
+    <row r="21" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="C21" s="3"/>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="3"/>
+      <c r="G21" s="3"/>
+      <c r="H21" s="3"/>
+      <c r="I21" s="3"/>
+    </row>
+    <row r="22" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="C22" s="3"/>
+      <c r="D22" s="3"/>
+      <c r="E22" s="3"/>
+      <c r="F22" s="3"/>
+      <c r="G22" s="3"/>
+      <c r="H22" s="3"/>
+      <c r="I22" s="3"/>
+    </row>
+    <row r="23" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="C23" s="3"/>
+      <c r="D23" s="3"/>
+      <c r="E23" s="3"/>
+      <c r="F23" s="3"/>
+      <c r="G23" s="3"/>
+      <c r="H23" s="3"/>
+      <c r="I23" s="3"/>
+    </row>
+    <row r="24" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="C24" s="3"/>
+      <c r="D24" s="3"/>
+      <c r="E24" s="3"/>
+      <c r="F24" s="3"/>
+      <c r="G24" s="3"/>
+      <c r="H24" s="3"/>
+      <c r="I24" s="3"/>
+    </row>
+    <row r="25" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="C25" s="3"/>
+      <c r="D25" s="3"/>
+      <c r="E25" s="3"/>
+      <c r="F25" s="3"/>
+      <c r="G25" s="3"/>
+      <c r="H25" s="3"/>
+      <c r="I25" s="3"/>
+    </row>
+    <row r="26" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="C26" s="3"/>
+      <c r="D26" s="3"/>
+      <c r="E26" s="3"/>
+      <c r="F26" s="3"/>
+      <c r="G26" s="3"/>
+      <c r="H26" s="3"/>
+      <c r="I26" s="3"/>
+    </row>
+    <row r="27" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="C27" s="3"/>
+      <c r="D27" s="3"/>
+      <c r="E27" s="3"/>
+      <c r="F27" s="3"/>
+      <c r="G27" s="3"/>
+      <c r="H27" s="3"/>
+      <c r="I27" s="3"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="C2:I2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>